<commit_message>
Updated typos in import files.
</commit_message>
<xml_diff>
--- a/import-files/adamig-1-0.xlsx
+++ b/import-files/adamig-1-0.xlsx
@@ -11,10 +11,10 @@
     <sheet name="adamig-1-0-compl" sheetId="13" r:id="rId2"/>
     <sheet name="adamig-1-0-ds" sheetId="2" r:id="rId3"/>
     <sheet name="adam-1-0-vg" sheetId="8" r:id="rId4"/>
-    <sheet name="adamig-1-0-de" sheetId="9" r:id="rId5"/>
+    <sheet name="adamig-1-0-col" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'adamig-1-0-de'!$A$1:$K$291</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'adamig-1-0-col'!$A$1:$K$291</definedName>
     <definedName name="IDX" localSheetId="2">'adamig-1-0-ds'!#REF!</definedName>
     <definedName name="sdtmig_3_1_2_export_00_model" localSheetId="0">'adamig-1-0'!$A$1:$D$2</definedName>
     <definedName name="sdtmig_3_1_2_export_00_model" localSheetId="1">'adamig-1-0-compl'!$A$1:$C$2</definedName>

</xml_diff>

<commit_message>
Added adam validation rules.
</commit_message>
<xml_diff>
--- a/import-files/adamig-1-0.xlsx
+++ b/import-files/adamig-1-0.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2697" uniqueCount="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="1243">
   <si>
     <t>ADAE</t>
   </si>
@@ -4799,19 +4799,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
@@ -4866,50 +4866,76 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>863</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>864</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C6" s="7">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>